<commit_message>
fixed comp_props issues and separated plotting
</commit_message>
<xml_diff>
--- a/example/name_to_properties/data_name_to_properties/checked_compounds_properties.xlsx
+++ b/example/name_to_properties/data_name_to_properties/checked_compounds_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/gcms_data_analysis/example/name_to_properties/data_name_to_properties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_1C4577905B70DA21FF392311595ED87656CDDA34" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D6EBF4F-4FDA-4B19-9675-87ACD127BBDD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_1C4577905B70DA21FF392311595ED87656CDDA34" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0EA78AC-AEF6-45D0-BFDF-02581EE47B37}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>canonical_smiles</t>
   </si>
@@ -188,6 +188,24 @@
   </si>
   <si>
     <t>comp_name</t>
+  </si>
+  <si>
+    <t>el_mf_Br</t>
+  </si>
+  <si>
+    <t>el_mf_C</t>
+  </si>
+  <si>
+    <t>el_mf_Cl</t>
+  </si>
+  <si>
+    <t>el_mf_H</t>
+  </si>
+  <si>
+    <t>el_mf_O</t>
+  </si>
+  <si>
+    <t>el_mf_Si</t>
   </si>
 </sst>
 </file>
@@ -550,19 +568,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:L9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.3125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -600,58 +620,76 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -674,73 +712,91 @@
         <v>0</v>
       </c>
       <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>0.74967231873504636</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>8.3886403828149381E-2</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>0.16643087485696451</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>3</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="U2">
+      <c r="AA2">
         <v>0.43775096223863519</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
         <v>0.59369603661708115</v>
       </c>
-      <c r="AC2">
+      <c r="AI2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -763,73 +819,91 @@
         <v>0</v>
       </c>
       <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>32</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0.74945792059901717</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>0.125793619842446</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>0.1247874580765931</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>15</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
         <v>1</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
         <v>0.82447936978394809</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>0.1755596287341081</v>
       </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -852,73 +926,91 @@
         <v>0</v>
       </c>
       <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>32</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>0.74945792059901717</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>0.125793619842446</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>0.1247874580765931</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>15</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>1</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
         <v>0.82447936978394809</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <v>0.1755596287341081</v>
       </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -941,73 +1033,91 @@
         <v>0</v>
       </c>
       <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>0.76576346828179798</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>6.4265221549250878E-2</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>0.17000318775900539</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>6</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>1</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
         <v>0.81931781957284022</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
         <v>0.18071405801721391</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -1030,73 +1140,91 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>0.36507598784194528</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>0.53875379939209733</v>
       </c>
-      <c r="J6">
+      <c r="P6">
         <v>1.531914893617021E-2</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>8.1048632218844979E-2</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>6</v>
       </c>
-      <c r="O6">
+      <c r="U6">
         <v>3</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>1</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
         <v>0.37528875379939208</v>
       </c>
-      <c r="W6">
+      <c r="AC6">
         <v>0.53875379939209733</v>
       </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
         <v>8.6155015197568394E-2</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1119,73 +1247,91 @@
         <v>0</v>
       </c>
       <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>0.65006314270250765</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>8.4863792170304889E-2</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>9.6211437849539963E-2</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>0.1688916952312226</v>
       </c>
-      <c r="M7">
+      <c r="S7">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="T7">
         <v>6</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>1</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
         <v>0.27124300920079381</v>
       </c>
-      <c r="V7">
+      <c r="AB7">
         <v>0.46368392567201883</v>
       </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
         <v>9.6211437849539963E-2</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
         <v>0.16886162727764739</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1205,76 +1351,94 @@
         <v>2.4</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>0.46184613606149932</v>
       </c>
-      <c r="H8">
+      <c r="N8">
         <v>0.41654239639327212</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>2.9131264088781E-2</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>9.2474423443731579E-2</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>6</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>1</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
         <v>0.43984740766429692</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
         <v>9.8300676261487793E-2</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <v>0.46185191607421539</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1297,73 +1461,91 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <v>57</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>104</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>0.77324034334763947</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>0.11840072283713569</v>
       </c>
-      <c r="K9">
+      <c r="Q9">
         <v>0.10841879376552969</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
         <v>51</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
         <v>3</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
         <v>0.80455500338829911</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
         <v>0.19550485656200589</v>
       </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>

</xml_diff>